<commit_message>
update RNN and added new model
</commit_message>
<xml_diff>
--- a/models/model-results.xlsx
+++ b/models/model-results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>benchmark</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>60.000-70.000</t>
+  </si>
+  <si>
+    <t>lstm128_lr1e-5</t>
+  </si>
+  <si>
+    <t>100-90.000</t>
+  </si>
+  <si>
+    <t>90.000-100.000</t>
   </si>
 </sst>
 </file>
@@ -567,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,14 +588,14 @@
     <col min="2" max="2" width="97.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="63.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="38.5703125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -605,28 +614,28 @@
         <v>0</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>17</v>
@@ -645,20 +654,20 @@
       <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>30</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -669,29 +678,29 @@
       <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>30</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>18</v>
@@ -711,34 +720,34 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>100</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -752,28 +761,66 @@
         <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>100</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>0.46619396782698302</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>0.83560466152964397</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0.44488209486007602</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>0.85869411930616202</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>15</v>
+    </row>
+    <row r="6" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1">
+        <v>300</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.43877539889849798</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.86418295996080696</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.38935984671115798</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.86938856406699005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new CNN model, new Tester.py, updated /pt and xlsx
</commit_message>
<xml_diff>
--- a/models/model-results.xlsx
+++ b/models/model-results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>benchmark</t>
   </si>
@@ -184,6 +184,17 @@
   <si>
     <t>type': '1-hot sequence-200 only Taken/NotTaken, no program counter',
 'batch_size': 64</t>
+  </si>
+  <si>
+    <t>RNNLayer(
+  (rnn): LSTM(2, 256, batch_first=True)
+  (normalization): BatchNorm1d(256, eps=1e-05, momentum=0.1, affine=True, track_running_stats=True)
+  (fc): Linear(in_features=256, out_features=2, bias=True)
+  (softmax): Softmax(dim=-1)
+)</t>
+  </si>
+  <si>
+    <t>lstm256_1layer</t>
   </si>
 </sst>
 </file>
@@ -594,12 +605,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +619,7 @@
     <col min="2" max="2" width="97.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
@@ -879,6 +890,44 @@
       </c>
       <c r="L7" s="1">
         <v>0.88395600039639199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1">
+        <v>150</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.43356797496053201</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.86986148844252398</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.37473037838935802</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.88068575958775097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>